<commit_message>
Anh khoa chạy lại 3 file SQLQueryBaoCaoDinhLuong.sql,SQLQueryTOnKhoTOng.sql, BaoCaoNgay.sql
</commit_message>
<xml_diff>
--- a/BaoCaoCongViec/BaoCao.xlsx
+++ b/BaoCaoCongViec/BaoCao.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MinhTien\SVN\trunk\BaoCaoCongViec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Minh Tien\KiemTien\Karaoke\BaoCaoCongViec\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Chức năng" sheetId="1" r:id="rId1"/>
     <sheet name="Report" sheetId="2" r:id="rId2"/>
+    <sheet name="Resize Ảnh" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="85">
   <si>
     <t>Khách hàng</t>
   </si>
@@ -211,6 +212,75 @@
   </si>
   <si>
     <t>Danh sách giá</t>
+  </si>
+  <si>
+    <t>Báo cáo lịch sử bán hàng</t>
+  </si>
+  <si>
+    <t>Báo cáo tồn kho</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Chiều rộng</t>
+  </si>
+  <si>
+    <t>Chiều cao</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Cai đặt bàn</t>
+  </si>
+  <si>
+    <t>Sơ đồ bàn</t>
+  </si>
+  <si>
+    <t>Cài đặt bàn</t>
+  </si>
+  <si>
+    <t>Cài đặt giao diện bán hàng</t>
+  </si>
+  <si>
+    <t>Các button chức năng</t>
+  </si>
+  <si>
+    <t>Cài đặt máy in</t>
+  </si>
+  <si>
+    <t>Máy in hóa đơn</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>Cài đặt thông tin doanh nghiệp</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Hình đại diện</t>
+  </si>
+  <si>
+    <t>Tất cả</t>
+  </si>
+  <si>
+    <t>Thức ăn</t>
+  </si>
+  <si>
+    <t>Nước</t>
+  </si>
+  <si>
+    <t>Cài đặt giao diện chức năng bán hàng</t>
+  </si>
+  <si>
+    <t>Cài đặt chức năng hiển thị</t>
+  </si>
+  <si>
+    <t>Cài đặt sơ đồ bàn</t>
   </si>
 </sst>
 </file>
@@ -259,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -282,11 +352,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,6 +391,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -594,17 +682,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -720,12 +808,24 @@
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -737,12 +837,22 @@
       <c r="B5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I5" s="9" t="s">
         <v>14</v>
       </c>
@@ -754,12 +864,22 @@
       <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I6" s="9" t="s">
         <v>14</v>
       </c>
@@ -810,12 +930,22 @@
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I10" s="9" t="s">
         <v>14</v>
       </c>
@@ -825,12 +955,22 @@
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I11" s="9" t="s">
         <v>14</v>
       </c>
@@ -842,12 +982,24 @@
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -855,12 +1007,22 @@
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I13" s="9" t="s">
         <v>14</v>
       </c>
@@ -870,12 +1032,22 @@
       <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I14" s="9" t="s">
         <v>14</v>
       </c>
@@ -941,12 +1113,22 @@
       <c r="B19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I19" s="9" t="s">
         <v>14</v>
       </c>
@@ -971,87 +1153,163 @@
       <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="C24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="C25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I26" s="9" t="s">
         <v>14</v>
       </c>
@@ -1059,97 +1317,165 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9" t="s">
-        <v>14</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9" t="s">
-        <v>14</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="I32" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -1157,12 +1483,16 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
+      <c r="I33" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+      <c r="A34" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -1173,11 +1503,9 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="A35" s="10"/>
       <c r="B35" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -1190,7 +1518,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1201,29 +1529,112 @@
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
+      <c r="A37" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="B37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A40:A42"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1232,12 +1643,420 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3">
+        <v>120</v>
+      </c>
+      <c r="D3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>1024</v>
+      </c>
+      <c r="D4">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="D12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <v>120</v>
+      </c>
+      <c r="D14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>